<commit_message>
path update (pg1, pg2)
</commit_message>
<xml_diff>
--- a/static/Certificate_Page1.xlsx
+++ b/static/Certificate_Page1.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Page1" sheetId="1" state="visible" r:id="rId1"/>
@@ -83,50 +83,50 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -196,6 +196,36 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1000125" cy="1000125"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,7 +512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -495,7 +525,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="9" min="9" width="14"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -796,8 +826,9 @@
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="H40:I40"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.5" right="0.75" top="1"/>
+  <pageMargins left="0.5" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperHeight="13in" paperWidth="8.5in"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -815,6 +846,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
page 1 and 2 backend
</commit_message>
<xml_diff>
--- a/static/Certificate_Page1.xlsx
+++ b/static/Certificate_Page1.xlsx
@@ -576,7 +576,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Legazpi City</t>
+          <t>Legazpi City, Albay</t>
         </is>
       </c>
       <c r="B4" s="3" t="n"/>
@@ -591,7 +591,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Tel No. (052) 481-7881</t>
+          <t>(052) 481-7881</t>
         </is>
       </c>
       <c r="B5" s="3" t="n"/>
@@ -719,7 +719,7 @@
     <row r="22">
       <c r="A22" s="7" t="inlineStr">
         <is>
-          <t>Issued this 14th day of June, 2010 upon the request of Ms. Lumbao for reference</t>
+          <t>Issued this 15th day of July, 2021 upon the request of Ms. Lumbao for reference</t>
         </is>
       </c>
       <c r="B22" s="8" t="n"/>

</xml_diff>